<commit_message>
* Added via tenting * Generated output files
</commit_message>
<xml_diff>
--- a/MIXR Input and Processing/Project Outputs for MIXR Input and Processing/MIXR Input and Processing_1.0.xlsx
+++ b/MIXR Input and Processing/Project Outputs for MIXR Input and Processing/MIXR Input and Processing_1.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Taiping\Documents\FYDP\mixr-hardware\MIXR Input and Processing\Project Outputs for MIXR Input and Processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B4F48CF-7FB6-43F2-BC66-9129BCA82B22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C1193AFA-AB0A-469E-8260-D74328E55904}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3045" yWindow="3780" windowWidth="28800" windowHeight="8220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="306">
   <si>
     <t>Title</t>
   </si>
@@ -111,7 +111,7 @@
     <t>Taiping Li</t>
   </si>
   <si>
-    <t>2020-02-03 8:42 PM</t>
+    <t>2020-02-08 7:17 PM</t>
   </si>
   <si>
     <t>1</t>
@@ -213,9 +213,6 @@
     <t>CONN 5POS 0.1" 1" MALE HEADER</t>
   </si>
   <si>
-    <t>CONN 3POS HEADR MALE 0.1"</t>
-  </si>
-  <si>
     <t>BJT NPN 40V 1.5A SOT-23</t>
   </si>
   <si>
@@ -309,7 +306,7 @@
     <t>C2, C3, C4, C5, C6, C7, C9, C10, C11, C13, C15, C16, C17, C18, C19, C20, C29, C37, C38, C41, C42, C45, C46, C54, C55, C58, C59, C62, C63, C66, C72, C73, C74, C75, C76, C77, C78, C80, C82, C85, C99, C100, C101, C102, C103, C104, C107, C108</t>
   </si>
   <si>
-    <t>C8, C39, C40, C43, C44, C56, C57, C60, C61</t>
+    <t>C8, C39, C40, C43, C44, C56, C57, C60, C61, C109</t>
   </si>
   <si>
     <t>C12, C14, C71</t>
@@ -390,9 +387,6 @@
     <t>P6, P7</t>
   </si>
   <si>
-    <t>P9, P10</t>
-  </si>
-  <si>
     <t>Q1, Q2</t>
   </si>
   <si>
@@ -402,7 +396,7 @@
     <t>R2, R3, R4, R5, R6, R39, R40, R43, R44</t>
   </si>
   <si>
-    <t>R7, R8, R20, R24, R25, R26, R27, R28, R30, R61, R67, R69</t>
+    <t>R7, R8, R20, R24, R25, R26, R27, R28, R30, R61, R67, R69, R72</t>
   </si>
   <si>
     <t>R10</t>
@@ -843,9 +837,6 @@
     <t>SAM9000-ND</t>
   </si>
   <si>
-    <t>732-5316-ND</t>
-  </si>
-  <si>
     <t>641-1790-1-ND</t>
   </si>
   <si>
@@ -948,10 +939,10 @@
     <t>Bill of Materials for Variant [Standard] of Project [MIXR Input and Processing.PrjPcb] (No PCB Document Selected)</t>
   </si>
   <si>
-    <t>8:42 PM</t>
-  </si>
-  <si>
-    <t>2020-02-03</t>
+    <t>7:17 PM</t>
+  </si>
+  <si>
+    <t>2020-02-08</t>
   </si>
   <si>
     <t>BOM_PartType</t>
@@ -1530,7 +1521,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:J72"/>
+  <dimension ref="A2:J71"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="L6" sqref="L6"/>
@@ -1636,28 +1627,28 @@
         <v>30</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F11" s="21" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G11" s="21" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="H11" s="21" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="I11" s="21" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -1665,28 +1656,28 @@
         <v>31</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="G12" s="3">
-        <v>2.58</v>
+        <v>2.59</v>
       </c>
       <c r="H12" s="3">
         <v>1</v>
       </c>
       <c r="I12" s="10">
-        <v>2.58</v>
+        <v>2.59</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -1694,28 +1685,28 @@
         <v>32</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="G13" s="3">
-        <v>5.0290000000000001E-2</v>
+        <v>5.0569999999999997E-2</v>
       </c>
       <c r="H13" s="3">
         <v>48</v>
       </c>
       <c r="I13" s="10">
-        <v>2.41</v>
+        <v>2.4300000000000002</v>
       </c>
     </row>
     <row r="14" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -1723,28 +1714,28 @@
         <v>33</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="G14" s="3">
-        <v>0.60877999999999999</v>
+        <v>0.42848000000000003</v>
       </c>
       <c r="H14" s="3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I14" s="10">
-        <v>5.48</v>
+        <v>4.28</v>
       </c>
     </row>
     <row r="15" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -1752,28 +1743,28 @@
         <v>34</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G15" s="3">
-        <v>0.58230999999999999</v>
+        <v>0.58550000000000002</v>
       </c>
       <c r="H15" s="3">
         <v>3</v>
       </c>
       <c r="I15" s="10">
-        <v>1.75</v>
+        <v>1.76</v>
       </c>
     </row>
     <row r="16" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -1781,28 +1772,28 @@
         <v>35</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G16" s="3">
-        <v>0.33085999999999999</v>
+        <v>0.33267000000000002</v>
       </c>
       <c r="H16" s="3">
         <v>7</v>
       </c>
       <c r="I16" s="10">
-        <v>2.3199999999999998</v>
+        <v>2.33</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -1810,28 +1801,28 @@
         <v>36</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G17" s="3">
-        <v>0.13234000000000001</v>
+        <v>0.13306999999999999</v>
       </c>
       <c r="H17" s="3">
         <v>2</v>
       </c>
       <c r="I17" s="10">
-        <v>0.26468999999999998</v>
+        <v>0.26613999999999999</v>
       </c>
     </row>
     <row r="18" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -1839,28 +1830,28 @@
         <v>37</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G18" s="3">
-        <v>0.29644999999999999</v>
+        <v>0.29807</v>
       </c>
       <c r="H18" s="3">
         <v>11</v>
       </c>
       <c r="I18" s="10">
-        <v>3.26</v>
+        <v>3.28</v>
       </c>
     </row>
     <row r="19" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -1868,28 +1859,28 @@
         <v>38</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G19" s="3">
-        <v>0.95286999999999999</v>
+        <v>0.95809999999999995</v>
       </c>
       <c r="H19" s="3">
         <v>2</v>
       </c>
       <c r="I19" s="10">
-        <v>1.91</v>
+        <v>1.92</v>
       </c>
     </row>
     <row r="20" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -1897,28 +1888,28 @@
         <v>39</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="G20" s="3">
-        <v>0.66171999999999997</v>
+        <v>0.66534000000000004</v>
       </c>
       <c r="H20" s="3">
         <v>4</v>
       </c>
       <c r="I20" s="10">
-        <v>2.65</v>
+        <v>2.66</v>
       </c>
     </row>
     <row r="21" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -1926,28 +1917,28 @@
         <v>40</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G21" s="3">
-        <v>1.56</v>
+        <v>1.57</v>
       </c>
       <c r="H21" s="3">
         <v>4</v>
       </c>
       <c r="I21" s="10">
-        <v>6.25</v>
+        <v>6.28</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -1955,28 +1946,28 @@
         <v>41</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="G22" s="3">
-        <v>0.15881000000000001</v>
+        <v>0.15967999999999999</v>
       </c>
       <c r="H22" s="3">
         <v>4</v>
       </c>
       <c r="I22" s="10">
-        <v>0.63524999999999998</v>
+        <v>0.63873000000000002</v>
       </c>
     </row>
     <row r="23" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -1984,28 +1975,28 @@
         <v>42</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G23" s="3">
-        <v>0.13234000000000001</v>
+        <v>0.13306999999999999</v>
       </c>
       <c r="H23" s="3">
         <v>2</v>
       </c>
       <c r="I23" s="10">
-        <v>0.26468999999999998</v>
+        <v>0.26613999999999999</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -2013,28 +2004,28 @@
         <v>43</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G24" s="3">
-        <v>0.13234000000000001</v>
+        <v>0.13306999999999999</v>
       </c>
       <c r="H24" s="3">
         <v>4</v>
       </c>
       <c r="I24" s="10">
-        <v>0.52937000000000001</v>
+        <v>0.53227999999999998</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -2042,22 +2033,22 @@
         <v>44</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G25" s="3">
-        <v>0.54261000000000004</v>
+        <v>0.54557999999999995</v>
       </c>
       <c r="H25" s="3">
         <v>2</v>
@@ -2071,28 +2062,28 @@
         <v>45</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="G26" s="3">
-        <v>0.25145000000000001</v>
+        <v>0.25283</v>
       </c>
       <c r="H26" s="3">
         <v>2</v>
       </c>
       <c r="I26" s="10">
-        <v>0.50290000000000001</v>
+        <v>0.50566</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -2100,28 +2091,28 @@
         <v>46</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="G27" s="3">
-        <v>0.25145000000000001</v>
+        <v>0.25283</v>
       </c>
       <c r="H27" s="3">
         <v>2</v>
       </c>
       <c r="I27" s="10">
-        <v>0.50290000000000001</v>
+        <v>0.50566</v>
       </c>
     </row>
     <row r="28" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -2129,28 +2120,28 @@
         <v>47</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="G28" s="3">
-        <v>0.68818000000000001</v>
+        <v>0.69196000000000002</v>
       </c>
       <c r="H28" s="3">
         <v>1</v>
       </c>
       <c r="I28" s="10">
-        <v>0.68818000000000001</v>
+        <v>0.69196000000000002</v>
       </c>
     </row>
     <row r="29" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -2158,28 +2149,28 @@
         <v>48</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="G29" s="3">
-        <v>0.62200999999999995</v>
+        <v>0.62541999999999998</v>
       </c>
       <c r="H29" s="3">
         <v>1</v>
       </c>
       <c r="I29" s="10">
-        <v>0.62200999999999995</v>
+        <v>0.62541999999999998</v>
       </c>
     </row>
     <row r="30" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -2187,28 +2178,28 @@
         <v>49</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="G30" s="3">
-        <v>0.63524999999999998</v>
+        <v>0.63873000000000002</v>
       </c>
       <c r="H30" s="3">
         <v>4</v>
       </c>
       <c r="I30" s="10">
-        <v>2.54</v>
+        <v>2.5499999999999998</v>
       </c>
     </row>
     <row r="31" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -2216,28 +2207,28 @@
         <v>50</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="G31" s="3">
-        <v>1.1100000000000001</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="H31" s="3">
         <v>1</v>
       </c>
       <c r="I31" s="10">
-        <v>1.1100000000000001</v>
+        <v>1.1200000000000001</v>
       </c>
     </row>
     <row r="32" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -2245,28 +2236,28 @@
         <v>51</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="G32" s="3">
-        <v>0.13234000000000001</v>
+        <v>0.13306999999999999</v>
       </c>
       <c r="H32" s="3">
         <v>1</v>
       </c>
       <c r="I32" s="10">
-        <v>0.13234000000000001</v>
+        <v>0.13306999999999999</v>
       </c>
     </row>
     <row r="33" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -2274,28 +2265,28 @@
         <v>52</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="G33" s="3">
-        <v>1.1499999999999999</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="H33" s="3">
         <v>1</v>
       </c>
       <c r="I33" s="10">
-        <v>1.1499999999999999</v>
+        <v>1.1599999999999999</v>
       </c>
     </row>
     <row r="34" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -2303,28 +2294,28 @@
         <v>53</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="G34" s="3">
-        <v>0.59553999999999996</v>
+        <v>0.59880999999999995</v>
       </c>
       <c r="H34" s="3">
         <v>3</v>
       </c>
       <c r="I34" s="10">
-        <v>1.79</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="35" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -2332,28 +2323,28 @@
         <v>54</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="G35" s="3">
-        <v>0.18528</v>
+        <v>0.18629999999999999</v>
       </c>
       <c r="H35" s="3">
         <v>3</v>
       </c>
       <c r="I35" s="10">
-        <v>0.55584</v>
+        <v>0.55889</v>
       </c>
     </row>
     <row r="36" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -2361,28 +2352,28 @@
         <v>55</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="G36" s="3">
-        <v>3.24</v>
+        <v>3.26</v>
       </c>
       <c r="H36" s="3">
         <v>1</v>
       </c>
       <c r="I36" s="10">
-        <v>3.24</v>
+        <v>3.26</v>
       </c>
     </row>
     <row r="37" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -2390,19 +2381,19 @@
         <v>56</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="G37" s="3"/>
       <c r="H37" s="3">
@@ -2415,28 +2406,28 @@
         <v>57</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="G38" s="3">
-        <v>2.94</v>
+        <v>2.95</v>
       </c>
       <c r="H38" s="3">
         <v>2</v>
       </c>
       <c r="I38" s="10">
-        <v>5.88</v>
+        <v>5.91</v>
       </c>
     </row>
     <row r="39" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -2444,28 +2435,28 @@
         <v>58</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G39" s="3">
-        <v>1.35</v>
+        <v>1.36</v>
       </c>
       <c r="H39" s="3">
         <v>1</v>
       </c>
       <c r="I39" s="10">
-        <v>1.35</v>
+        <v>1.36</v>
       </c>
     </row>
     <row r="40" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -2473,28 +2464,28 @@
         <v>59</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="G40" s="3">
-        <v>0.59553999999999996</v>
+        <v>0.59880999999999995</v>
       </c>
       <c r="H40" s="3">
         <v>2</v>
       </c>
       <c r="I40" s="10">
-        <v>1.19</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="41" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -2502,28 +2493,28 @@
         <v>60</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="D41" s="3">
-        <v>61300311121</v>
+        <v>166</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>207</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F41" s="9" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="G41" s="3">
-        <v>0.17205000000000001</v>
+        <v>0.29275000000000001</v>
       </c>
       <c r="H41" s="3">
         <v>2</v>
       </c>
       <c r="I41" s="10">
-        <v>0.34409000000000001</v>
+        <v>0.58550000000000002</v>
       </c>
     </row>
     <row r="42" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -2531,28 +2522,28 @@
         <v>61</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F42" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G42" s="3">
-        <v>0.29115000000000002</v>
+        <v>2.129E-2</v>
       </c>
       <c r="H42" s="3">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="I42" s="10">
-        <v>0.58230999999999999</v>
+        <v>0.31936999999999999</v>
       </c>
     </row>
     <row r="43" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -2560,28 +2551,28 @@
         <v>62</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F43" s="9" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G43" s="3">
-        <v>2.1170000000000001E-2</v>
+        <v>0.13306999999999999</v>
       </c>
       <c r="H43" s="3">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="I43" s="10">
-        <v>0.31762000000000001</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="44" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -2589,28 +2580,28 @@
         <v>63</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F44" s="9" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="G44" s="3">
-        <v>0.13234000000000001</v>
+        <v>3.0609999999999998E-2</v>
       </c>
       <c r="H44" s="3">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="I44" s="10">
-        <v>1.19</v>
+        <v>0.39788000000000001</v>
       </c>
     </row>
     <row r="45" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -2618,28 +2609,28 @@
         <v>64</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F45" s="9" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="G45" s="3">
-        <v>3.0439999999999998E-2</v>
+        <v>0.13306999999999999</v>
       </c>
       <c r="H45" s="3">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="I45" s="10">
-        <v>0.36526999999999998</v>
+        <v>0.13306999999999999</v>
       </c>
     </row>
     <row r="46" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -2647,28 +2638,28 @@
         <v>65</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>154</v>
+        <v>167</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F46" s="9" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="G46" s="3">
-        <v>0.13234000000000001</v>
+        <v>0.13306999999999999</v>
       </c>
       <c r="H46" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I46" s="10">
-        <v>0.13234000000000001</v>
+        <v>0.66534000000000004</v>
       </c>
     </row>
     <row r="47" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -2676,28 +2667,28 @@
         <v>66</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>169</v>
+        <v>152</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F47" s="9" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="G47" s="3">
-        <v>0.13234000000000001</v>
+        <v>0.13306999999999999</v>
       </c>
       <c r="H47" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I47" s="10">
-        <v>0.66171999999999997</v>
+        <v>0.26613999999999999</v>
       </c>
     </row>
     <row r="48" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -2705,28 +2696,28 @@
         <v>67</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F48" s="9" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="G48" s="3">
-        <v>0.13234000000000001</v>
+        <v>0.51897000000000004</v>
       </c>
       <c r="H48" s="3">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="I48" s="10">
-        <v>0.26468999999999998</v>
+        <v>4.1500000000000004</v>
       </c>
     </row>
     <row r="49" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -2734,28 +2725,28 @@
         <v>68</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F49" s="9" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="G49" s="3">
-        <v>0.51614000000000004</v>
+        <v>0.13306999999999999</v>
       </c>
       <c r="H49" s="3">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="I49" s="10">
-        <v>4.13</v>
+        <v>0.39921000000000001</v>
       </c>
     </row>
     <row r="50" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -2763,28 +2754,28 @@
         <v>69</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>154</v>
+        <v>167</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F50" s="9" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="G50" s="3">
-        <v>0.13234000000000001</v>
+        <v>0.13306999999999999</v>
       </c>
       <c r="H50" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I50" s="10">
-        <v>0.39702999999999999</v>
+        <v>0.13306999999999999</v>
       </c>
     </row>
     <row r="51" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -2792,28 +2783,28 @@
         <v>70</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F51" s="9" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="G51" s="3">
-        <v>0.13234000000000001</v>
+        <v>0.33267000000000002</v>
       </c>
       <c r="H51" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I51" s="10">
-        <v>0.13234000000000001</v>
+        <v>0.66534000000000004</v>
       </c>
     </row>
     <row r="52" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -2821,28 +2812,28 @@
         <v>71</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F52" s="9" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="G52" s="3">
-        <v>0.33085999999999999</v>
+        <v>0.54557999999999995</v>
       </c>
       <c r="H52" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I52" s="10">
-        <v>0.66171999999999997</v>
+        <v>2.1800000000000002</v>
       </c>
     </row>
     <row r="53" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -2850,28 +2841,28 @@
         <v>72</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F53" s="9" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="G53" s="3">
-        <v>0.54261000000000004</v>
+        <v>0.15967999999999999</v>
       </c>
       <c r="H53" s="3">
         <v>4</v>
       </c>
       <c r="I53" s="10">
-        <v>2.17</v>
+        <v>0.63873000000000002</v>
       </c>
     </row>
     <row r="54" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -2879,28 +2870,28 @@
         <v>73</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F54" s="9" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="G54" s="3">
-        <v>0.15881000000000001</v>
+        <v>0.38590000000000002</v>
       </c>
       <c r="H54" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I54" s="10">
-        <v>0.63524999999999998</v>
+        <v>0.38590000000000002</v>
       </c>
     </row>
     <row r="55" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -2908,28 +2899,28 @@
         <v>74</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F55" s="9" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="G55" s="3">
-        <v>0.38379000000000002</v>
+        <v>0.14638000000000001</v>
       </c>
       <c r="H55" s="3">
         <v>1</v>
       </c>
       <c r="I55" s="10">
-        <v>0.38379000000000002</v>
+        <v>0.14638000000000001</v>
       </c>
     </row>
     <row r="56" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -2937,28 +2928,28 @@
         <v>75</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F56" s="9" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="G56" s="3">
-        <v>0.14557999999999999</v>
+        <v>0.13306999999999999</v>
       </c>
       <c r="H56" s="3">
         <v>1</v>
       </c>
       <c r="I56" s="10">
-        <v>0.14557999999999999</v>
+        <v>0.13306999999999999</v>
       </c>
     </row>
     <row r="57" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -2966,28 +2957,28 @@
         <v>76</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>154</v>
+        <v>168</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F57" s="9" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G57" s="3">
-        <v>0.13234000000000001</v>
+        <v>0.26613999999999999</v>
       </c>
       <c r="H57" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I57" s="10">
-        <v>0.13234000000000001</v>
+        <v>0.79840999999999995</v>
       </c>
     </row>
     <row r="58" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -2995,28 +2986,28 @@
         <v>77</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F58" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="G58" s="3">
-        <v>0.26468999999999998</v>
+        <v>5.0599999999999996</v>
       </c>
       <c r="H58" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I58" s="10">
-        <v>0.79405999999999999</v>
+        <v>5.0599999999999996</v>
       </c>
     </row>
     <row r="59" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -3024,28 +3015,28 @@
         <v>78</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F59" s="9" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G59" s="3">
-        <v>5.03</v>
+        <v>0.94479000000000002</v>
       </c>
       <c r="H59" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I59" s="10">
-        <v>5.03</v>
+        <v>1.89</v>
       </c>
     </row>
     <row r="60" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -3053,28 +3044,28 @@
         <v>79</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F60" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="G60" s="3">
-        <v>0.93964000000000003</v>
+        <v>1.86</v>
       </c>
       <c r="H60" s="3">
         <v>2</v>
       </c>
       <c r="I60" s="10">
-        <v>1.88</v>
+        <v>3.73</v>
       </c>
     </row>
     <row r="61" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -3082,28 +3073,28 @@
         <v>80</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>173</v>
+        <v>155</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F61" s="9" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G61" s="3">
-        <v>1.85</v>
+        <v>16.89</v>
       </c>
       <c r="H61" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I61" s="10">
-        <v>3.71</v>
+        <v>16.89</v>
       </c>
     </row>
     <row r="62" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -3111,28 +3102,28 @@
         <v>81</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>157</v>
+        <v>172</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F62" s="9" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G62" s="3">
-        <v>16.79</v>
+        <v>4.43</v>
       </c>
       <c r="H62" s="3">
         <v>1</v>
       </c>
       <c r="I62" s="10">
-        <v>16.79</v>
+        <v>4.43</v>
       </c>
     </row>
     <row r="63" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -3140,28 +3131,28 @@
         <v>82</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F63" s="9" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="G63" s="3">
-        <v>4.41</v>
+        <v>13.11</v>
       </c>
       <c r="H63" s="3">
         <v>1</v>
       </c>
       <c r="I63" s="10">
-        <v>4.41</v>
+        <v>13.11</v>
       </c>
     </row>
     <row r="64" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -3169,28 +3160,28 @@
         <v>83</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F64" s="9" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="G64" s="3">
-        <v>13.04</v>
+        <v>3.55</v>
       </c>
       <c r="H64" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I64" s="10">
-        <v>13.04</v>
+        <v>7.11</v>
       </c>
     </row>
     <row r="65" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -3198,28 +3189,28 @@
         <v>84</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F65" s="9" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="G65" s="3">
-        <v>3.53</v>
+        <v>2.85</v>
       </c>
       <c r="H65" s="3">
         <v>2</v>
       </c>
       <c r="I65" s="10">
-        <v>7.07</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="66" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -3227,28 +3218,28 @@
         <v>85</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F66" s="9" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="G66" s="3">
-        <v>2.83</v>
+        <v>0.74519000000000002</v>
       </c>
       <c r="H66" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I66" s="10">
-        <v>5.66</v>
+        <v>0.74519000000000002</v>
       </c>
     </row>
     <row r="67" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -3256,28 +3247,28 @@
         <v>86</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F67" s="9" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G67" s="3">
-        <v>0.74112</v>
+        <v>1.61</v>
       </c>
       <c r="H67" s="3">
         <v>1</v>
       </c>
       <c r="I67" s="10">
-        <v>0.74112</v>
+        <v>1.61</v>
       </c>
     </row>
     <row r="68" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -3285,77 +3276,60 @@
         <v>87</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F68" s="9" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="G68" s="3">
-        <v>1.6</v>
+        <v>0.90486999999999995</v>
       </c>
       <c r="H68" s="3">
         <v>1</v>
       </c>
       <c r="I68" s="10">
-        <v>1.6</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="E69" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="F69" s="9" t="s">
-        <v>298</v>
-      </c>
-      <c r="G69" s="3">
-        <v>0.89993000000000001</v>
-      </c>
-      <c r="H69" s="3">
-        <v>1</v>
-      </c>
-      <c r="I69" s="10">
-        <v>0.89993000000000001</v>
+        <v>0.90486999999999995</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A69" s="11"/>
+      <c r="B69" s="12"/>
+      <c r="C69" s="26"/>
+      <c r="D69" s="12"/>
+      <c r="E69" s="12"/>
+      <c r="F69" s="13"/>
+      <c r="G69" s="12"/>
+      <c r="H69" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I69" s="14">
+        <f>SUM(I12:I68)</f>
+        <v>126.08141999999998</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A70" s="11"/>
-      <c r="B70" s="12"/>
-      <c r="C70" s="26"/>
-      <c r="D70" s="12"/>
-      <c r="E70" s="12"/>
-      <c r="F70" s="13"/>
-      <c r="G70" s="12"/>
-      <c r="H70" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I70" s="14">
-        <f>SUM(I12:I69)</f>
-        <v>126.91936999999997</v>
-      </c>
+      <c r="A70" s="15"/>
+      <c r="B70" s="16"/>
+      <c r="C70" s="16"/>
+      <c r="D70" s="15"/>
+      <c r="E70" s="15"/>
+      <c r="F70" s="15"/>
+      <c r="G70" s="15"/>
+      <c r="H70" s="15"/>
+      <c r="I70" s="15"/>
+      <c r="J70" s="17"/>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A71" s="15"/>
+      <c r="A71" s="16"/>
       <c r="B71" s="16"/>
       <c r="C71" s="16"/>
       <c r="D71" s="15"/>
@@ -3365,18 +3339,6 @@
       <c r="H71" s="15"/>
       <c r="I71" s="15"/>
       <c r="J71" s="17"/>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A72" s="16"/>
-      <c r="B72" s="16"/>
-      <c r="C72" s="16"/>
-      <c r="D72" s="15"/>
-      <c r="E72" s="15"/>
-      <c r="F72" s="15"/>
-      <c r="G72" s="15"/>
-      <c r="H72" s="15"/>
-      <c r="I72" s="15"/>
-      <c r="J72" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3416,7 +3378,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="18" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3432,7 +3394,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="18" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3448,7 +3410,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="6" spans="1:2" s="18" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3456,7 +3418,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="7" spans="1:2" s="18" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3472,7 +3434,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="9" spans="1:2" s="18" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3480,7 +3442,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="10" spans="1:2" s="18" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3504,7 +3466,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="32" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="13" spans="1:2" s="18" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3512,7 +3474,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="32" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="14" spans="1:2" s="18" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
* Regenerated PDF * Fixed vias
</commit_message>
<xml_diff>
--- a/MIXR Input and Processing/Project Outputs for MIXR Input and Processing/MIXR Input and Processing_1.0.xlsx
+++ b/MIXR Input and Processing/Project Outputs for MIXR Input and Processing/MIXR Input and Processing_1.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Taiping\Documents\FYDP\mixr-hardware\MIXR Input and Processing\Project Outputs for MIXR Input and Processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C1193AFA-AB0A-469E-8260-D74328E55904}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{247FD857-1178-4685-B0B6-1D964595E0B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3045" yWindow="3780" windowWidth="28800" windowHeight="8220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -111,7 +111,7 @@
     <t>Taiping Li</t>
   </si>
   <si>
-    <t>2020-02-08 7:17 PM</t>
+    <t>2020-02-09 8:54 PM</t>
   </si>
   <si>
     <t>1</t>
@@ -939,10 +939,10 @@
     <t>Bill of Materials for Variant [Standard] of Project [MIXR Input and Processing.PrjPcb] (No PCB Document Selected)</t>
   </si>
   <si>
-    <t>7:17 PM</t>
-  </si>
-  <si>
-    <t>2020-02-08</t>
+    <t>8:54 PM</t>
+  </si>
+  <si>
+    <t>2020-02-09</t>
   </si>
   <si>
     <t>BOM_PartType</t>

</xml_diff>